<commit_message>
Fixed a lot of errors
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -143,9 +143,6 @@
     <t>display personnalized purchase history //</t>
   </si>
   <si>
-    <t xml:space="preserve"> display users items currently for sale</t>
-  </si>
-  <si>
     <t>can display the items image // created the list template // page displays the listings containing the items and sellers info</t>
   </si>
   <si>
@@ -158,7 +155,10 @@
     <t>clears the input in the search bar  // must also reset the search result</t>
   </si>
   <si>
-    <t>make button disabled it nothing was searched</t>
+    <t>make button disabled if nothing was searched</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> display only users items currently for sale</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="60" customHeight="1"/>
@@ -684,7 +684,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" customHeight="1">
@@ -694,10 +694,9 @@
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="60" customHeight="1">
       <c r="A4" s="6" t="s">
@@ -715,12 +714,11 @@
         <v>33</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" customHeight="1">
@@ -734,10 +732,10 @@
     </row>
     <row r="7" spans="1:5" ht="60" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -783,11 +781,11 @@
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" customHeight="1">

</xml_diff>

<commit_message>
Worked on front end
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="main menu" sheetId="2" r:id="rId2"/>
-    <sheet name="account page" sheetId="5" r:id="rId3"/>
-    <sheet name="listing an item" sheetId="6" r:id="rId4"/>
+    <sheet name="listing an item" sheetId="6" r:id="rId3"/>
+    <sheet name="account page" sheetId="5" r:id="rId4"/>
     <sheet name="log functions" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>FONTEND</t>
   </si>
@@ -101,9 +101,6 @@
     <t>details button</t>
   </si>
   <si>
-    <t>details button must lead to a page containing the details of the item being sold</t>
-  </si>
-  <si>
     <t>buy button</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>return button works // adds to the global listing</t>
   </si>
   <si>
-    <t>display personnalized purchase history //</t>
-  </si>
-  <si>
     <t>can display the items image // created the list template // page displays the listings containing the items and sellers info</t>
   </si>
   <si>
@@ -152,13 +146,10 @@
     <t>list updates with every change to it</t>
   </si>
   <si>
-    <t>clears the input in the search bar  // must also reset the search result</t>
-  </si>
-  <si>
-    <t>make button disabled if nothing was searched</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> display only users items currently for sale</t>
+    <t>display personnalized purchase history //  display only users items currently for sale</t>
+  </si>
+  <si>
+    <t>clears the input in the search bar  // must also reset the search result // make button disabled if nothing was searched</t>
   </si>
 </sst>
 </file>
@@ -649,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="60" customHeight="1"/>
@@ -680,62 +671,60 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" customHeight="1">
       <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -746,10 +735,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="60" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="25.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="60" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="60" customHeight="1"/>
@@ -781,11 +853,8 @@
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" customHeight="1">
@@ -806,7 +875,7 @@
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -817,95 +886,9 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="6" spans="1:5" ht="60" customHeight="1">
       <c r="A6" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="60" customHeight="1"/>
-  <cols>
-    <col min="1" max="16384" width="25.7109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="60" customHeight="1">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="60" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="60" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>